<commit_message>
Add data about hospitals in Hanoi
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BKHN\Chous_Projects\Introduction_to_Data_Science\IDS-CapstoneProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2BF2F2-386F-4E3A-91B1-E6B39C3A35ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3338CC98-409B-4879-BA0F-EE5360099C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{97102754-A2DE-4C2B-9E5A-B0068D735524}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{97102754-A2DE-4C2B-9E5A-B0068D735524}"/>
   </bookViews>
   <sheets>
     <sheet name="RestaurantData" sheetId="1" r:id="rId1"/>
     <sheet name="RealEstateData" sheetId="2" r:id="rId2"/>
     <sheet name="PopulationData" sheetId="3" r:id="rId3"/>
     <sheet name="Schools" sheetId="5" r:id="rId4"/>
-    <sheet name="RestaurantCategories" sheetId="4" r:id="rId5"/>
+    <sheet name="Hospitals" sheetId="6" r:id="rId5"/>
+    <sheet name="RestaurantCategories" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5521" uniqueCount="4548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5775" uniqueCount="4789">
   <si>
     <t>Name</t>
   </si>
@@ -13734,6 +13735,729 @@
   </si>
   <si>
     <t>Đường Uy nỗ, Thị trấn Đông Anh, Đông Anh, Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Hữu Nghị</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN MẮT SÀI GÒN – HÀ NỘI</t>
+  </si>
+  <si>
+    <t>Bệnh viện Phụ sản Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Châm Cứu Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>Bệnh viện Phổi Hà Nội – Trung tâm chống Lao Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Bệnh Nhiệt Đới Trung Ương –  DANH SÁCH CÁC BỆNH VIỆN Ở TP HÀ NỘI</t>
+  </si>
+  <si>
+    <t>Tên bệnh viện</t>
+  </si>
+  <si>
+    <t>Fax.</t>
+  </si>
+  <si>
+    <t>Phone.</t>
+  </si>
+  <si>
+    <t>Điện Thoại: (024) 3942 9999  – 096 227 91 15</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN ĐA KHOA MÊ LINH</t>
+  </si>
+  <si>
+    <t>–  DANH SÁCH CÁC BỆNH VIỆN TẠI HÀ NỘI</t>
+  </si>
+  <si>
+    <t>Email: cskh@benhvienphusananthinh.vn</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 02433.825.059</t>
+  </si>
+  <si>
+    <t>Email: bvmhd@hanoi.gov.vn</t>
+  </si>
+  <si>
+    <t>Website:  http://mathadong.com/</t>
+  </si>
+  <si>
+    <t>Phone. 1800 1165 – 094 727 66 55</t>
+  </si>
+  <si>
+    <t>Email: tuvan@mathanoi2.vn</t>
+  </si>
+  <si>
+    <t>Website:  https://mathanoi2.vn/</t>
+  </si>
+  <si>
+    <t>Bệnh viện Mắt kỹ thuật cao Hà Nội</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 7778 6868</t>
+  </si>
+  <si>
+    <t>Email: cskh@benhvienmat.vn</t>
+  </si>
+  <si>
+    <t>Website:  https://mathitec.vn/ </t>
+  </si>
+  <si>
+    <t>Bệnh viện Mắt Quốc Tế DND</t>
+  </si>
+  <si>
+    <t>–  DANH SÁCH CÁC BỆNH VIỆN Ở HÀ NỘI</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 096 912 81 28</t>
+  </si>
+  <si>
+    <t>Phone. 096 912 81 28</t>
+  </si>
+  <si>
+    <t>Email: info@matquocte.vn</t>
+  </si>
+  <si>
+    <t>Website:   http://matquocte.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3974 8307</t>
+  </si>
+  <si>
+    <t>Email: info@matvietnhat.com.vn</t>
+  </si>
+  <si>
+    <t>Website: http://matvietnhat.com.vn/  </t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024.3755 8688 – 024.3756 6617</t>
+  </si>
+  <si>
+    <t>Email: tuvan@matvietnga.com</t>
+  </si>
+  <si>
+    <t>Website: http://matvietnga.com/ </t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 2240 1011</t>
+  </si>
+  <si>
+    <t>Email: tanduc74@yahoo.com</t>
+  </si>
+  <si>
+    <t>Website:  http://www.matanhsang.com</t>
+  </si>
+  <si>
+    <t>Điện Thoại:  024 3715 3666</t>
+  </si>
+  <si>
+    <t>Điện Thoại:  0243 728 0888 – 1900 55 88 96 hoặc 0904 97 0909</t>
+  </si>
+  <si>
+    <t>Phone.0904 97 0909</t>
+  </si>
+  <si>
+    <t>Email:  contact@thucuchospital.vn -cskh@zinniacorp.com</t>
+  </si>
+  <si>
+    <t>Website:  https://benhvienthucuc.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3974 3556</t>
+  </si>
+  <si>
+    <t>Website: https://www.vinmec.com/  </t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3927 5568</t>
+  </si>
+  <si>
+    <t>Email: info@hongngochospital.vn</t>
+  </si>
+  <si>
+    <t>Website:  http://hongngochospital.vn/</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Thẩm Mỹ Kangnam Hàn Quốc</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 7300 6466</t>
+  </si>
+  <si>
+    <t>Website: https://benhvienthammykangnam.vn/  </t>
+  </si>
+  <si>
+    <t>Email: cskh@benhvientriduc.vn</t>
+  </si>
+  <si>
+    <t>Website:  http://benhvientriduc.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3577 1100</t>
+  </si>
+  <si>
+    <t>Email: contact@hfh.com.vn</t>
+  </si>
+  <si>
+    <t>Website:  https://www.hfh.com.vn</t>
+  </si>
+  <si>
+    <t>quận Hoàng Mai, thành phố Hà Nội –  024 3224 7765 / 024 3640 2308</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3976 4463</t>
+  </si>
+  <si>
+    <t>Email:  info@buudienhospital.vn</t>
+  </si>
+  <si>
+    <t>Website: http://buudienhospital.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024.62504455</t>
+  </si>
+  <si>
+    <t>Website:   http://www.benhvienphusananthinh.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 1900 565656</t>
+  </si>
+  <si>
+    <t>Email: info@medlatec.com</t>
+  </si>
+  <si>
+    <t>Website:   https://medlatec.vn/</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3765 5599</t>
+  </si>
+  <si>
+    <t>Email: info@benhvienhathanh.vn</t>
+  </si>
+  <si>
+    <t>Website:  http://benhvienhathanh.vn/</t>
+  </si>
+  <si>
+    <t>Sở Y Tế Hà Nội</t>
+  </si>
+  <si>
+    <t>Điện Thoại: 024 3998 5765</t>
+  </si>
+  <si>
+    <t>Email: vanthu_soyt@hanoi.gov.vn</t>
+  </si>
+  <si>
+    <t>Website:  https://soyte.hanoi.gov.vn/</t>
+  </si>
+  <si>
+    <t>Bệnh viện Bạch Mai</t>
+  </si>
+  <si>
+    <t>Bệnh viện E, Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện tai mũi họng Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh Viện y học cổ truyền  Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện nội tiết Trung Ương Hà Nội </t>
+  </si>
+  <si>
+    <t>Bệnh viện K</t>
+  </si>
+  <si>
+    <t>Bệnh viện Việt Đức</t>
+  </si>
+  <si>
+    <t>Bệnh viện Nhi Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>78 Đường Giải Phóng, Phương Mai, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>87 – 89 đường Trần Cung, phường Nghĩa Tân, Quận Cầu Giấy, Hà Nội – Việt Nam</t>
+  </si>
+  <si>
+    <t>40 Tràng Thi, Hàng Bông, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>78 Giải Phóng, Phương Đình, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>85 Phố Bà Triệu, Bùi Thị Xuân, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>29 Nguyễn Bỉnh Khiêm, Nguyễn Du, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngõ 215 Đường Ngọc Hồi, Tứ Hiệp, Thanh Trì, Hà Nội; 80 Ngõ 82 Yên Lãng, Láng Hạ, Đống Đa, Hà Nội,</t>
+  </si>
+  <si>
+    <t>43 Quán Sứ, Hàng Bông, Hoàn Kiếm, Hà Nội; Tựu Liệt, Tam Hiệp, Thanh Trì, Hà Nội; Số 30 đường Tân Triều, Cầu Bươu, Thanh Trì, Hà Nội.</t>
+  </si>
+  <si>
+    <t>40 Tràng Thi, Hàng Bông, Hoàn Kiếm Hà Nội</t>
+  </si>
+  <si>
+    <t>43 Tràng Thi, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>18/879 Đường La Thành, Láng Thượng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>49 Thái Thịnh, Láng Hạ, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 463, đường Hoàng Hoa Thám, quận Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>192 Nguyễn Lương Bằng, Quận Đống Đa , Hà Nội</t>
+  </si>
+  <si>
+    <t>42 Thanh Nhàn, Quỳnh Mai, Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>12 Chu Văn An, Điện Bàn, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>37 Hai Bà Trưng, Tràng Tiền, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>Tổ 18 – thị trấn Đông Anh – Huyện Đông Anh – Hà Nội, Đông Anh, Hà Nội</t>
+  </si>
+  <si>
+    <t>42A Thanh Nhàn, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>Xã Hòa Bình, Huyện Thường Tín, Hoà Binh, Thường Tín, Hà Nội</t>
+  </si>
+  <si>
+    <t>Ngõ 467 Nguyễn Văn Linh – P.Sài Đồng – Q.Long Biên – TP. Hà Nội</t>
+  </si>
+  <si>
+    <t>SỐ 44 THANH NHÀN, Quận Hai Bà Trưng, Hà Nội.</t>
+  </si>
+  <si>
+    <t>37, Phố Hai Bà Trưng, Phường Tràng Tiền, Quận Hoàn Kiếm, Thành Phố Hà Nội</t>
+  </si>
+  <si>
+    <t>Km3 Tiên Dương, Tiên Dương, Đông Anh, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>118 Tứ Hiệp, Văn Điển, Thanh Trì, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Phù Linh, Sóc Sơn, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>1B1 Tập thể Bệnh viện giao thông vận tải, Láng Thượng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>263 Đường Phùng Hưng – Quận Hà Đông – Thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>15A – Phương Mai – Quận Đống Đa – Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 1 phố Yec Xanh, Phạm Đình Hổ, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>261 Phùng Hưng, P. Phúc La, Hà Đông, Hà Nội</t>
+  </si>
+  <si>
+    <t>9 Trần Bình, Mai Dịch, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>TL80, Phúc Lâm, Mỹ Đức, Hà Nội</t>
+  </si>
+  <si>
+    <t>70 Nguyễn Chí Thanh, Láng Thượng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>2 Trần Phú, P. Mộ Lao, Hà Đông, P. Mộ Lao Hà Đông Hà Nội</t>
+  </si>
+  <si>
+    <t>99 Nguyễn Viết Xuân, P. Quang Trung, Hà Đông, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Cao Lỗ, Uy Nỗ, Đông Anh, Hà Nội</t>
+  </si>
+  <si>
+    <t>54 Trường Lâm, Đức Giang, Long Biên, Hà Nội</t>
+  </si>
+  <si>
+    <t>Thị Trấn Phùng – Đan Phượng – Hà nội</t>
+  </si>
+  <si>
+    <t>Thôn Lũng Kênh, Đức Giang, Hoài Đức, Hà Nội</t>
+  </si>
+  <si>
+    <t>Thôn 1, xã Thạch Đà, huyện Mê Linh, TP. Hà Nội</t>
+  </si>
+  <si>
+    <t>Tổ dân phố Thọ Sơn, thị trấn Đại Nghĩa, huyện Mỹ Đức, thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>TT. Quốc Oai, Quốc Oai, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 79, đường 420, xã Kim Quan, huyện Thạch Thất, TP.Hà Nội</t>
+  </si>
+  <si>
+    <t>115 Trần Phú, TT. Thường Tín, Thường Tín, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>20 Bế Văn Đàn, P. Quang Trung, Hà Đông, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Ba Thá Viên An Huyện Ứng Hoà, Viên An, Ứng Hòa, Hà Nội</t>
+  </si>
+  <si>
+    <t>2D Nguyễn Viết Xuân, P. Quang Trung, Q. Hà Đông, Tp Hà Nội</t>
+  </si>
+  <si>
+    <t>72 Nguyễn Chí Thanh, Phường Láng Thượng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>128 Bùi Thị Xuân, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>122 Triệu Việt Vương, Bùi Thị Xuân, Hai Bà Trưng, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>2 Trần Cung, Cổ Nhuế, Từ Liêm, Hà Nội</t>
+  </si>
+  <si>
+    <t>286 Thụy Khuê, Bưởi, Tây Hồ, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Số 55 Yên Ninh,Trúc Bạch, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>61 Vũ Thạnh, Chợ Dừa, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>4 Sơn Tây, Điện Bàn, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện đa khoa Đống Đa</t>
+  </si>
+  <si>
+    <t>Bênh viện Ung bướu Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Tâm thần trung ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Trung tâm Y tế Sóc Sơn</t>
+  </si>
+  <si>
+    <t>Bệnh viện Y học Cổ truyền trung ương</t>
+  </si>
+  <si>
+    <t>Bệnh Viện lão khoa Trung Ương </t>
+  </si>
+  <si>
+    <t>Bệnh viện Thanh Nhàn</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Răng Hàm Mặt Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện mắt Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Lao và bệnh phổi Trung Ương Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Bắc Thăng Long</t>
+  </si>
+  <si>
+    <t>Bệnh viện Giao thông vận tải trung ương</t>
+  </si>
+  <si>
+    <t>Viện huyết học truyền máu trung ương</t>
+  </si>
+  <si>
+    <t>Viện sức khỏe tâm thần Quốc Gia</t>
+  </si>
+  <si>
+    <t>Bệnh viện đa khoa Xanh–Pôn</t>
+  </si>
+  <si>
+    <t>Bệnh viện Hữu nghị Việt Nam – Cu ba</t>
+  </si>
+  <si>
+    <t>Bệnh viện tâm thần Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Đa khoa Huyện Hoài Đức</t>
+  </si>
+  <si>
+    <t>Bệnh viện phụ sản Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Mắt Hà Nội – Trung tâm mắt Hà Nội</t>
+  </si>
+  <si>
+    <t>Trung tâm y tế Gia Lâm</t>
+  </si>
+  <si>
+    <t>Trung tâm y tế Đông Anh</t>
+  </si>
+  <si>
+    <t>Trung tâm Y tế huyện Thanh Trì</t>
+  </si>
+  <si>
+    <t>Bệnh viện Đa khoa Nông Nghiệp</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Da Liễu Trung Ương</t>
+  </si>
+  <si>
+    <t>Bệnh Viện bỏng quốc gia Lê Hữu Trác</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Thận Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Đông Anh</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Đức Giang</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Huyện Đan Phượng</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Huyện Quốc Oai</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Huyện Thạch Thất</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Mắt Hà Đông</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN PHỤ SẢN AN THỊNH</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN ĐA KHOA TƯ NHÂN HÀ THÀNH</t>
+  </si>
+  <si>
+    <t>Viện tim mạch trung ương Hà Nội –  Viện tim mạch việt nam</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN TIM HÀ NỘI</t>
+  </si>
+  <si>
+    <t>VIỆN VỆ SINH DỊCH TỄ TRUNG ƯƠNG</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Nam Thăng Long</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Sóc Sơn</t>
+  </si>
+  <si>
+    <t>Bệnh Viện đa khoa Huyện Ba Vì</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Huyện Thường Tín</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Da Liễu Hà Nội</t>
+  </si>
+  <si>
+    <t>Bệnh viện Mắt Việt Nhật</t>
+  </si>
+  <si>
+    <t>Bệnh viện mắt quốc tế Nhật Bản</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Quốc Tế Thu Cúc</t>
+  </si>
+  <si>
+    <t>Bệnh viện Đa khoa Quốc tế Vinmec Times City</t>
+  </si>
+  <si>
+    <t>Bệnh viện Đa khoa Hồng Ngọc</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN QUÂN Y 103</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN 19 – 8 BỘ CÔNG AN VIỆT NAM</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN TRUNG ƯƠNG QUÂN ĐỘI 108</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN XÂY DỰNG</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Y Học Cổ Truyền Hà Đông</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Quận Hà Đông</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Sơn Tây</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Hòe Nhai 2</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Chương Mỹ</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa khoa Huyện Mỹ Đức</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa khoa Huyện Phúc Thọ</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Đa Khoa Huyện Thanh Oai</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Tâm Thần Ba Thá</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Mắt Hà Nội 2</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Mắt Quốc Tế Việt – Nga</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Mắt Ánh Sáng</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN ĐA KHOA TRÍ ĐỨC</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN VIỆT PHÁP HÀ NỘI</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Tâm Thần Mỹ Đức</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Tuệ Tĩnh</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Da Liễu Hà Đông</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN BƯU ĐIỆN HÀ NỘI</t>
+  </si>
+  <si>
+    <t>BỆNH VIỆN ĐA KHOA MEDLATEC HÀ NỘI</t>
+  </si>
+  <si>
+    <t>1 Trần Khánh Dư, Bạch Đằng, Hai Bà Trưng, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">929 Đường La Thành, Láng Thượng, Ba Đình, Hà Nội; Số 38, Cảm Hội, Hai Bà Trưng, Hà Nội;  Số 10, Đường Quang Trung, Hà Đông, Hà Nội </t>
+  </si>
+  <si>
+    <t>Số 3 Ngô Xuân Quảng, Trâu Quỳ, Gia Lâm, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Km13+500, Quốc lộ 1A, Ngọc Hồi, Thanh Trì, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Phạm Văn Bạch, Yên Hoà, Cầu Giấy, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>1A Phương Mai, Đống Đa, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>78 Giải Phóng, Phương Đình, Đống Đa, Hà Nội Việt Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78 Giải Phóng, Phương Đình, Đống Đa, Hà Nội, Việt Nam; Thôn Bầu, xã Kim Chung, huyện Đông Anh, thành phố Hà Nội </t>
+  </si>
+  <si>
+    <t>92 Trần Hưng Đạo, Phường Cửa Nam, Quận Hoàn Kiếm, Hà Nội; Đường Võ Chí Công, Quận Tây Hồ, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 1 Trần Hưng Đạo, Bạch Đằng, Hai Bà Trưng, Hà Nội  </t>
+  </si>
+  <si>
+    <t>Nguyễn Quý Đức, Thanh Xuân Bắc, Hà Nội</t>
+  </si>
+  <si>
+    <t> 38 Tân Xuân, Xuân Đỉnh, Bắc Từ Liêm, Hà Nội</t>
+  </si>
+  <si>
+    <t> 2 Bế Văn Đàn, P. Quang Trung, Hà Đông, P. Quang Trung Hà Đông Hà Nội</t>
+  </si>
+  <si>
+    <t> Số 18 Đường Bệnh Viện, Tiên Dược, Sóc Sơn, Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 304A, đường Lê Lợi, P. Lê Lợi, Sơn Tây, Hà Nội</t>
+  </si>
+  <si>
+    <t>53 Tân Ấp, Phúc xá, Ba Đình, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>Xã Đồng Thái, huyện Ba Vì, thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t> 120 ĐT419, Ngọc Hoà , Chương Mỹ, Hà Nội</t>
+  </si>
+  <si>
+    <t>Phúc Hoà, Phúc Thọ, Hà Nội</t>
+  </si>
+  <si>
+    <t> TT. Kim Bài, Thanh Oai, Hà Nội</t>
+  </si>
+  <si>
+    <t>51-53-55 Trần Nhân Tông, Bùi Thị Xuân, Hà Nội</t>
+  </si>
+  <si>
+    <t>Nhà C2, Làng Quốc Tế Thăng Long, Dịch Vọng, quận Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>32 Phó Đức Chính, Trúc Bạch, Ba Đình, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>458 Phố Minh Khai, Vĩnh Tuy, Hai Bà Trưng, Hà Nội, Việt Nam</t>
+  </si>
+  <si>
+    <t>190 Trường Chinh, Khương Thượng, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>219 Đường Lê Duẩn, Nguyễn Du, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t> 1 Phương Mai, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Yên Bái II, Phố Huế, Hai Bà Trưng, Hà Nội –  024 3224 7765</t>
+  </si>
+  <si>
+    <t>Số 49 phố Trần Điền, phường Định Công,</t>
+  </si>
+  <si>
+    <t>496 Bạch Mai – Hai Bà Trưng, phường Trương Định thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t>42 Nghĩa Dũng, Phúc xá, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>79B Phố Nguyễn Khuyến, Văn Miếu, Đống Đa, Hà Nội , Việt Nam; Số 20 Bế Văn Đàn – Hà Đông – Hà Nội; Khoa Điều trị Nội trú Quốc Oai – Quốc Oai – Hà Nội</t>
+  </si>
+  <si>
+    <t>số 532 Đường Láng, Q. Đống Đa, Tp. Hà Nội; số 77 Nguyễn Du, quận Hai Bà Trưng, Tp. Hà Nội</t>
   </si>
 </sst>
 </file>
@@ -14258,14 +14982,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -14276,6 +14995,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -14285,7 +15010,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14618,38 +15342,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="G2" s="40"/>
       <c r="K2" t="s">
         <v>12</v>
       </c>
@@ -15706,7 +16430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BE72FB-5A39-4E70-A3DD-C0F58D41C610}">
   <dimension ref="A1:Q1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O52" workbookViewId="0">
+    <sheetView topLeftCell="O52" workbookViewId="0">
       <selection activeCell="U63" sqref="U63"/>
     </sheetView>
   </sheetViews>
@@ -15772,7 +16496,7 @@
       <c r="M3" t="s">
         <v>4278</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="39" t="s">
         <v>4279</v>
       </c>
       <c r="P3" t="s">
@@ -15811,7 +16535,7 @@
       <c r="M4" t="s">
         <v>4287</v>
       </c>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="39" t="s">
         <v>4280</v>
       </c>
       <c r="P4" t="s">
@@ -16464,7 +17188,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="30">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="41" t="s">
         <v>268</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -16484,7 +17208,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="30">
-      <c r="A27" s="43"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="18" t="s">
         <v>270</v>
       </c>
@@ -16502,7 +17226,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A28" s="44"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="18" t="s">
         <v>271</v>
       </c>
@@ -23259,10 +23983,10 @@
       <c r="H475" s="31" t="s">
         <v>1119</v>
       </c>
-      <c r="J475" s="40" t="s">
+      <c r="J475" s="44" t="s">
         <v>3485</v>
       </c>
-      <c r="K475" s="40" t="s">
+      <c r="K475" s="44" t="s">
         <v>3486</v>
       </c>
     </row>
@@ -23285,8 +24009,8 @@
       <c r="H476" s="31" t="s">
         <v>3483</v>
       </c>
-      <c r="J476" s="41"/>
-      <c r="K476" s="41"/>
+      <c r="J476" s="45"/>
+      <c r="K476" s="45"/>
     </row>
     <row r="477" spans="1:11" ht="17.25" thickBot="1">
       <c r="A477" s="20" t="s">
@@ -26733,10 +27457,10 @@
       <c r="H688" s="20" t="s">
         <v>1453</v>
       </c>
-      <c r="J688" s="40" t="s">
+      <c r="J688" s="44" t="s">
         <v>3819</v>
       </c>
-      <c r="K688" s="40" t="s">
+      <c r="K688" s="44" t="s">
         <v>3820</v>
       </c>
     </row>
@@ -26759,8 +27483,8 @@
       <c r="H689" s="20" t="s">
         <v>1451</v>
       </c>
-      <c r="J689" s="41"/>
-      <c r="K689" s="41"/>
+      <c r="J689" s="45"/>
+      <c r="K689" s="45"/>
     </row>
     <row r="690" spans="1:11" ht="15.75" thickBot="1">
       <c r="A690" s="16" t="s">
@@ -33020,10 +33744,10 @@
       <c r="H1017" s="20" t="s">
         <v>1983</v>
       </c>
-      <c r="J1017" s="40" t="s">
+      <c r="J1017" s="44" t="s">
         <v>4269</v>
       </c>
-      <c r="K1017" s="40" t="s">
+      <c r="K1017" s="44" t="s">
         <v>4270</v>
       </c>
     </row>
@@ -33046,8 +33770,8 @@
       <c r="H1018" s="20" t="s">
         <v>4223</v>
       </c>
-      <c r="J1018" s="41"/>
-      <c r="K1018" s="41"/>
+      <c r="J1018" s="45"/>
+      <c r="K1018" s="45"/>
     </row>
     <row r="1019" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1019" s="17" t="s">
@@ -33068,10 +33792,10 @@
       <c r="H1019" s="20" t="s">
         <v>4225</v>
       </c>
-      <c r="J1019" s="40" t="s">
+      <c r="J1019" s="44" t="s">
         <v>4271</v>
       </c>
-      <c r="K1019" s="40" t="s">
+      <c r="K1019" s="44" t="s">
         <v>4272</v>
       </c>
     </row>
@@ -33094,8 +33818,8 @@
       <c r="H1020" s="20" t="s">
         <v>4227</v>
       </c>
-      <c r="J1020" s="41"/>
-      <c r="K1020" s="41"/>
+      <c r="J1020" s="45"/>
+      <c r="K1020" s="45"/>
     </row>
     <row r="1021" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1021" s="17" t="s">
@@ -33501,15 +34225,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="J1019:J1020"/>
+    <mergeCell ref="K1019:K1020"/>
+    <mergeCell ref="J688:J689"/>
+    <mergeCell ref="K688:K689"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="J475:J476"/>
     <mergeCell ref="K475:K476"/>
     <mergeCell ref="J1017:J1018"/>
     <mergeCell ref="K1017:K1018"/>
-    <mergeCell ref="J1019:J1020"/>
-    <mergeCell ref="K1019:K1020"/>
-    <mergeCell ref="J688:J689"/>
-    <mergeCell ref="K688:K689"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D17" r:id="rId1" display="http://hghanoi.edu.vn/" xr:uid="{2AB6CB4A-666B-497B-9CF3-DA528DA179F1}"/>
@@ -33520,6 +34244,1111 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEBA3C5-3A11-44D8-BC17-E47D5EE3A816}">
+  <dimension ref="B1:C177"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>4621</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4629</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>4548</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>4622</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>4692</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4631</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>4623</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>4693</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>4624</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>4625</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>4626</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>4627</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>4549</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4788</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>4550</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4638</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>4628</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4639</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>4551</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>4694</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4641</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>4685</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>4691</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>4699</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>4700</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>4695</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>4686</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>4687</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4648</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>4703</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>4701</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4649</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>4553</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>4704</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4651</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>4705</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>4706</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
+        <v>4707</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4653</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>4688</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4654</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
+        <v>4696</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4655</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" t="s">
+        <v>4708</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>4689</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
+        <v>4710</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>4709</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4657</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
+        <v>4697</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>4690</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>4698</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>4720</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>4554</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>4721</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4764</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
+        <v>4722</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>4733</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>4734</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
+        <v>4735</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
+        <v>4736</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4766</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
+        <v>4723</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>4751</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>4711</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>4752</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>4737</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4664</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>4738</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>4724</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" t="s">
+        <v>4739</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" t="s">
+        <v>4712</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4665</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>4713</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>4740</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" t="s">
+        <v>4725</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4772</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>4741</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>4714</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>4702</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4668</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>4559</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" t="s">
+        <v>4742</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" t="s">
+        <v>4743</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>4715</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>4716</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4672</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
+        <v>4744</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>4726</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4673</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" t="s">
+        <v>4753</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" t="s">
+        <v>4745</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>4727</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4787</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" t="s">
+        <v>4555</v>
+      </c>
+      <c r="C84" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" t="s">
+        <v>4717</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4676</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="C86" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="C87" t="s">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="C88" t="s">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="C89" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" t="s">
+        <v>4746</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4677</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="C91" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="C92" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="C93" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" t="s">
+        <v>4568</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4776</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" t="s">
+        <v>4560</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="C96" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="C97" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" t="s">
+        <v>4572</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4678</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" t="s">
+        <v>4573</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="C100" t="s">
+        <v>4575</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="C101" t="s">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3">
+      <c r="C102" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3">
+      <c r="B103" t="s">
+        <v>4728</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3">
+      <c r="C104" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3">
+      <c r="C105" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3">
+      <c r="C106" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
+      <c r="B107" t="s">
+        <v>4747</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
+      <c r="C108" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3">
+      <c r="C109" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
+      <c r="C110" t="s">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3">
+      <c r="C111" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3">
+      <c r="B112" t="s">
+        <v>4748</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="C113" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="C114" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="C115" t="s">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3">
+      <c r="C116" t="s">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" t="s">
+        <v>4729</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3">
+      <c r="C119" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3">
+      <c r="C120" t="s">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3">
+      <c r="C121" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="C122" t="s">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
+      <c r="C123" t="s">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3">
+      <c r="B124" t="s">
+        <v>4730</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3">
+      <c r="C126" t="s">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="C127" t="s">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3">
+      <c r="C128" t="s">
+        <v>4589</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3">
+      <c r="C129" t="s">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3">
+      <c r="C130" t="s">
+        <v>4591</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3">
+      <c r="B132" t="s">
+        <v>4731</v>
+      </c>
+      <c r="C132" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3">
+      <c r="C133" t="s">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3">
+      <c r="C134" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3">
+      <c r="C135" t="s">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3">
+      <c r="C136" t="s">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137" t="s">
+        <v>4732</v>
+      </c>
+      <c r="C137" t="s">
+        <v>4682</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3">
+      <c r="C138" t="s">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3">
+      <c r="C139" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3">
+      <c r="C140" t="s">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3">
+      <c r="C141" t="s">
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3">
+      <c r="B142" t="s">
+        <v>4597</v>
+      </c>
+      <c r="C142" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3">
+      <c r="B143" t="s">
+        <v>4560</v>
+      </c>
+      <c r="C143" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3">
+      <c r="C144" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="C145" t="s">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3">
+      <c r="C146" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3">
+      <c r="B147" t="s">
+        <v>4749</v>
+      </c>
+      <c r="C147" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3">
+      <c r="C148" t="s">
+        <v>4558</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3">
+      <c r="C149" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="C150" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3">
+      <c r="C151" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3">
+      <c r="B152" t="s">
+        <v>4750</v>
+      </c>
+      <c r="C152" t="s">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3">
+      <c r="C153" t="s">
+        <v>4602</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3">
+      <c r="C154" t="s">
+        <v>4603</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3">
+      <c r="C155" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3">
+      <c r="B156" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C156" t="s">
+        <v>4783</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3">
+      <c r="C157" t="s">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3">
+      <c r="C158" t="s">
+        <v>4605</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3">
+      <c r="C159" t="s">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3">
+      <c r="C160" t="s">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3">
+      <c r="C161" t="s">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3">
+      <c r="C162" t="s">
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3">
+      <c r="B163" t="s">
+        <v>4718</v>
+      </c>
+      <c r="C163" t="s">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3">
+      <c r="C164" t="s">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3">
+      <c r="C165" t="s">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3">
+      <c r="B166" t="s">
+        <v>4755</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4786</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3">
+      <c r="C167" t="s">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3">
+      <c r="C168" t="s">
+        <v>4612</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3">
+      <c r="C169" t="s">
+        <v>4613</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3">
+      <c r="B170" t="s">
+        <v>4719</v>
+      </c>
+      <c r="C170" t="s">
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3">
+      <c r="C171" t="s">
+        <v>4614</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3">
+      <c r="C172" t="s">
+        <v>4615</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3">
+      <c r="C173" t="s">
+        <v>4616</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3">
+      <c r="B174" t="s">
+        <v>4617</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4684</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3">
+      <c r="C175" t="s">
+        <v>4618</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3">
+      <c r="C176" t="s">
+        <v>4619</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3">
+      <c r="C177" t="s">
+        <v>4620</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC5E29-4737-4065-9887-48BBD6081583}">
   <dimension ref="A1:O32"/>
   <sheetViews>
@@ -33626,7 +35455,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -33673,7 +35502,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1">
-      <c r="A5" s="46"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="9" t="s">
         <v>51</v>
       </c>
@@ -33718,7 +35547,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="39" thickBot="1">
-      <c r="A6" s="46"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="9" t="s">
         <v>62</v>
       </c>
@@ -33763,7 +35592,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A7" s="46"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="9" t="s">
         <v>72</v>
       </c>
@@ -33808,7 +35637,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="9" t="s">
         <v>83</v>
       </c>
@@ -33853,7 +35682,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="9" t="s">
         <v>72</v>
       </c>
@@ -33898,7 +35727,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="9" t="s">
         <v>100</v>
       </c>
@@ -33941,7 +35770,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="9" t="s">
         <v>108</v>
       </c>
@@ -33980,7 +35809,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="9" t="s">
         <v>117</v>
       </c>
@@ -34017,7 +35846,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="9" t="s">
         <v>125</v>
       </c>
@@ -34052,7 +35881,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="39" thickBot="1">
-      <c r="A14" s="46"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="9" t="s">
         <v>131</v>
       </c>
@@ -34087,7 +35916,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1">
-      <c r="A15" s="46"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="9" t="s">
         <v>45</v>
       </c>
@@ -34118,7 +35947,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A16" s="46"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="9" t="s">
         <v>142</v>
       </c>
@@ -34147,7 +35976,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" thickBot="1">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="9" t="s">
         <v>75</v>
       </c>
@@ -34174,7 +36003,7 @@
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="9" t="s">
         <v>151</v>
       </c>
@@ -34201,7 +36030,7 @@
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1">
-      <c r="A19" s="46"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="9" t="s">
         <v>154</v>
       </c>
@@ -34226,7 +36055,7 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" ht="26.25" thickBot="1">
-      <c r="A20" s="46"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -34247,7 +36076,7 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1">
-      <c r="A21" s="46"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -34268,7 +36097,7 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1">
-      <c r="A22" s="46"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -34289,7 +36118,7 @@
       <c r="O22" s="9"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1">
-      <c r="A23" s="46"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -34310,7 +36139,7 @@
       <c r="O23" s="9"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -34331,7 +36160,7 @@
       <c r="O24" s="9"/>
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>

</xml_diff>